<commit_message>
Updated the test data and updated locators
</commit_message>
<xml_diff>
--- a/AutomationFramework/src/test/resources/TestData/TestData.xlsx
+++ b/AutomationFramework/src/test/resources/TestData/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDE2F8AD-FF9E-42F0-8F59-BFF5AF313E7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B683A5FA-28C9-497C-90F5-0CC7EEF2D9CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="131">
   <si>
     <t>TestCases</t>
   </si>
@@ -359,12 +359,6 @@
     <t>Ross</t>
   </si>
   <si>
-    <t>admin@at.com</t>
-  </si>
-  <si>
-    <t>114477@88</t>
-  </si>
-  <si>
     <t>Mr</t>
   </si>
   <si>
@@ -419,9 +413,6 @@
     <t>8844117720</t>
   </si>
   <si>
-    <t>newtest@mail.com</t>
-  </si>
-  <si>
     <t>23651</t>
   </si>
   <si>
@@ -431,13 +422,25 @@
     <t>223336655</t>
   </si>
   <si>
-    <t>newTester1@tmail.com</t>
-  </si>
-  <si>
-    <t>newTester2@tmail.com</t>
-  </si>
-  <si>
-    <t>newTester3@tmail.com</t>
+    <t>admin@testing.com</t>
+  </si>
+  <si>
+    <t>truetesting@123</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>newtester@tmail.com</t>
+  </si>
+  <si>
+    <t>newTester1@kmail.com</t>
+  </si>
+  <si>
+    <t>newTester2@kmail.com</t>
+  </si>
+  <si>
+    <t>newTester3@kmail.com</t>
   </si>
 </sst>
 </file>
@@ -904,7 +907,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -1256,16 +1259,16 @@
         <v>99</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="H2" s="11" t="s">
         <v>71</v>
       </c>
       <c r="I2" s="11" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="J2" s="11" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="K2" s="11" t="s">
         <v>101</v>
@@ -1281,13 +1284,13 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" customWidth="1"/>
     <col min="4" max="4" width="17.7109375" customWidth="1"/>
     <col min="5" max="5" width="17.28515625" customWidth="1"/>
@@ -1303,10 +1306,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>103</v>
+        <v>124</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>104</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -1339,7 +1342,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -1356,7 +1359,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1376,8 +1379,8 @@
       <c r="A2" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="B2" s="11">
-        <v>2</v>
+      <c r="B2" s="11" t="s">
+        <v>126</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>47</v>
@@ -1489,34 +1492,34 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>62</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E2" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="G2" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="H2" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="I2" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="J2" s="11" t="s">
         <v>118</v>
-      </c>
-      <c r="I2" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>120</v>
       </c>
       <c r="K2" s="11" t="s">
         <v>68</v>
@@ -1525,45 +1528,45 @@
         <v>99</v>
       </c>
       <c r="M2" s="11" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="N2" s="11" t="s">
         <v>71</v>
       </c>
       <c r="O2" s="11" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B3" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="D3" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="E3" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="F3" s="11" t="s">
         <v>106</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>108</v>
       </c>
       <c r="G3" s="11" t="s">
         <v>65</v>
       </c>
       <c r="H3" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="J3" s="11" t="s">
         <v>109</v>
-      </c>
-      <c r="I3" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="J3" s="11" t="s">
-        <v>111</v>
       </c>
       <c r="K3" s="11" t="s">
         <v>68</v>
@@ -1572,18 +1575,18 @@
         <v>69</v>
       </c>
       <c r="M3" s="11" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="N3" s="11" t="s">
         <v>71</v>
       </c>
       <c r="O3" s="11" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>62</v>

</xml_diff>